<commit_message>
Add result files for the show_results tests
</commit_message>
<xml_diff>
--- a/tests/results/result_test_show_results_all.xlsx
+++ b/tests/results/result_test_show_results_all.xlsx
@@ -27,34 +27,34 @@
     <t>Monat</t>
   </si>
   <si>
+    <t>Startguthaben</t>
+  </si>
+  <si>
+    <t>Endsaldo</t>
+  </si>
+  <si>
+    <t>Investitionen</t>
+  </si>
+  <si>
+    <t>Tilgungszahlungen</t>
+  </si>
+  <si>
+    <t>Rückkäufe</t>
+  </si>
+  <si>
+    <t>Zinszahlungen</t>
+  </si>
+  <si>
+    <t>Zinszahlungen aus Rückkäufen</t>
+  </si>
+  <si>
+    <t>Verzugsgebühren</t>
+  </si>
+  <si>
     <t>Ausfälle</t>
   </si>
   <si>
-    <t>Endsaldo</t>
-  </si>
-  <si>
     <t>Gesamteinnahmen</t>
-  </si>
-  <si>
-    <t>Investitionen</t>
-  </si>
-  <si>
-    <t>Rückkäufe</t>
-  </si>
-  <si>
-    <t>Startguthaben</t>
-  </si>
-  <si>
-    <t>Tilgungszahlungen</t>
-  </si>
-  <si>
-    <t>Verzugsgebühren</t>
-  </si>
-  <si>
-    <t>Zinszahlungen</t>
-  </si>
-  <si>
-    <t>Zinszahlungen aus Rückkäufen</t>
   </si>
   <si>
     <t>Bondora</t>
@@ -520,29 +520,29 @@
         <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>-12.43</v>
+        <v>1.19</v>
       </c>
       <c r="E2" t="n">
         <v>0.7</v>
       </c>
       <c r="F2" t="n">
-        <v>159.37</v>
+        <v>-455</v>
       </c>
       <c r="G2" t="n">
-        <v>-455</v>
+        <v>282.71</v>
       </c>
       <c r="H2" t="s"/>
       <c r="I2" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="J2" t="n">
-        <v>282.71</v>
-      </c>
+        <v>171.8</v>
+      </c>
+      <c r="J2" t="s"/>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>171.8</v>
-      </c>
-      <c r="M2" t="s"/>
+        <v>-12.43</v>
+      </c>
+      <c r="M2" t="n">
+        <v>159.37</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="n"/>
@@ -551,29 +551,29 @@
         <v>16</v>
       </c>
       <c r="D3" t="n">
-        <v>-18.63</v>
+        <v>0.7</v>
       </c>
       <c r="E3" t="n">
         <v>19.6</v>
       </c>
       <c r="F3" t="n">
-        <v>145.75</v>
+        <v>-1411</v>
       </c>
       <c r="G3" t="n">
-        <v>-1411</v>
+        <v>265.51</v>
       </c>
       <c r="H3" t="s"/>
       <c r="I3" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="J3" t="n">
-        <v>265.51</v>
-      </c>
+        <v>164.38</v>
+      </c>
+      <c r="J3" t="s"/>
       <c r="K3" t="s"/>
       <c r="L3" t="n">
-        <v>164.38</v>
-      </c>
-      <c r="M3" t="s"/>
+        <v>-18.63</v>
+      </c>
+      <c r="M3" t="n">
+        <v>145.75</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="n"/>
@@ -582,29 +582,29 @@
         <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>-44.74</v>
+        <v>19.6</v>
       </c>
       <c r="E4" t="n">
         <v>5.7</v>
       </c>
       <c r="F4" t="n">
-        <v>121.84</v>
+        <v>-419</v>
       </c>
       <c r="G4" t="n">
-        <v>-419</v>
+        <v>238.52</v>
       </c>
       <c r="H4" t="s"/>
       <c r="I4" t="n">
-        <v>19.6</v>
-      </c>
-      <c r="J4" t="n">
-        <v>238.52</v>
-      </c>
+        <v>166.58</v>
+      </c>
+      <c r="J4" t="s"/>
       <c r="K4" t="s"/>
       <c r="L4" t="n">
-        <v>166.58</v>
-      </c>
-      <c r="M4" t="s"/>
+        <v>-44.74</v>
+      </c>
+      <c r="M4" t="n">
+        <v>121.84</v>
+      </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="n"/>
@@ -613,29 +613,29 @@
         <v>18</v>
       </c>
       <c r="D5" t="n">
-        <v>-41.6</v>
+        <v>5.7</v>
       </c>
       <c r="E5" t="n">
         <v>0.77</v>
       </c>
       <c r="F5" t="n">
-        <v>149.5</v>
+        <v>-385</v>
       </c>
       <c r="G5" t="n">
-        <v>-385</v>
+        <v>188.97</v>
       </c>
       <c r="H5" t="s"/>
       <c r="I5" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="J5" t="n">
-        <v>188.97</v>
-      </c>
+        <v>191.1</v>
+      </c>
+      <c r="J5" t="s"/>
       <c r="K5" t="s"/>
       <c r="L5" t="n">
-        <v>191.1</v>
-      </c>
-      <c r="M5" t="s"/>
+        <v>-41.6</v>
+      </c>
+      <c r="M5" t="n">
+        <v>149.5</v>
+      </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
@@ -650,21 +650,21 @@
       <c r="D6" t="s"/>
       <c r="E6" t="s"/>
       <c r="F6" t="n">
+        <v>-2830</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2830</v>
+      </c>
+      <c r="H6" t="s"/>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="G6" t="n">
-        <v>-2830</v>
-      </c>
-      <c r="H6" t="s"/>
-      <c r="I6" t="s"/>
-      <c r="J6" t="n">
-        <v>2830</v>
-      </c>
+      <c r="J6" t="s"/>
       <c r="K6" t="s"/>
-      <c r="L6" t="n">
+      <c r="L6" t="s"/>
+      <c r="M6" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="s"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="n"/>
@@ -675,21 +675,21 @@
       <c r="D7" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="n">
+        <v>-2670</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2670</v>
+      </c>
+      <c r="H7" t="s"/>
+      <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="G7" t="n">
-        <v>-2670</v>
-      </c>
-      <c r="H7" t="s"/>
-      <c r="I7" t="s"/>
-      <c r="J7" t="n">
-        <v>2670</v>
-      </c>
+      <c r="J7" t="s"/>
       <c r="K7" t="s"/>
-      <c r="L7" t="n">
+      <c r="L7" t="s"/>
+      <c r="M7" t="n">
         <v>0</v>
       </c>
-      <c r="M7" t="s"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="n"/>
@@ -700,21 +700,21 @@
       <c r="D8" t="s"/>
       <c r="E8" t="s"/>
       <c r="F8" t="n">
+        <v>-2330</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4390</v>
+      </c>
+      <c r="H8" t="s"/>
+      <c r="I8" t="n">
         <v>122.37</v>
       </c>
-      <c r="G8" t="n">
-        <v>-2330</v>
-      </c>
-      <c r="H8" t="s"/>
-      <c r="I8" t="s"/>
-      <c r="J8" t="n">
-        <v>4390</v>
-      </c>
+      <c r="J8" t="s"/>
       <c r="K8" t="s"/>
-      <c r="L8" t="n">
+      <c r="L8" t="s"/>
+      <c r="M8" t="n">
         <v>122.37</v>
       </c>
-      <c r="M8" t="s"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="n"/>
@@ -725,21 +725,21 @@
       <c r="D9" t="s"/>
       <c r="E9" t="s"/>
       <c r="F9" t="n">
+        <v>-500</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1520</v>
+      </c>
+      <c r="H9" t="s"/>
+      <c r="I9" t="n">
         <v>60.65</v>
       </c>
-      <c r="G9" t="n">
-        <v>-500</v>
-      </c>
-      <c r="H9" t="s"/>
-      <c r="I9" t="s"/>
-      <c r="J9" t="n">
-        <v>1520</v>
-      </c>
+      <c r="J9" t="s"/>
       <c r="K9" t="s"/>
-      <c r="L9" t="n">
+      <c r="L9" t="s"/>
+      <c r="M9" t="n">
         <v>60.65</v>
       </c>
-      <c r="M9" t="s"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="n"/>
@@ -756,15 +756,15 @@
         <v>0</v>
       </c>
       <c r="H10" t="s"/>
-      <c r="I10" t="s"/>
-      <c r="J10" t="n">
+      <c r="I10" t="n">
         <v>0</v>
       </c>
+      <c r="J10" t="s"/>
       <c r="K10" t="s"/>
-      <c r="L10" t="n">
+      <c r="L10" t="s"/>
+      <c r="M10" t="n">
         <v>0</v>
       </c>
-      <c r="M10" t="s"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
@@ -776,26 +776,30 @@
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s"/>
-      <c r="E11" t="s"/>
+      <c r="D11" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="E11" t="n">
+        <v>43.56</v>
+      </c>
       <c r="F11" t="n">
-        <v>9.77</v>
+        <v>-50</v>
       </c>
       <c r="G11" t="n">
-        <v>-50</v>
+        <v>78.5</v>
       </c>
       <c r="H11" t="s"/>
-      <c r="I11" t="s"/>
-      <c r="J11" t="n">
-        <v>28.5</v>
-      </c>
+      <c r="I11" t="n">
+        <v>10.18</v>
+      </c>
+      <c r="J11" t="s"/>
       <c r="K11" t="n">
         <v>0.01</v>
       </c>
-      <c r="L11" t="n">
-        <v>9.76</v>
-      </c>
-      <c r="M11" t="s"/>
+      <c r="L11" t="s"/>
+      <c r="M11" t="n">
+        <v>10.19</v>
+      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="n"/>
@@ -803,26 +807,30 @@
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s"/>
-      <c r="E12" t="s"/>
+      <c r="D12" t="n">
+        <v>43.56</v>
+      </c>
+      <c r="E12" t="n">
+        <v>28.51</v>
+      </c>
       <c r="F12" t="n">
-        <v>16.73</v>
+        <v>-200</v>
       </c>
       <c r="G12" t="n">
-        <v>-200</v>
+        <v>168.71</v>
       </c>
       <c r="H12" t="s"/>
-      <c r="I12" t="s"/>
-      <c r="J12" t="n">
-        <v>18.71</v>
-      </c>
+      <c r="I12" t="n">
+        <v>16.24</v>
+      </c>
+      <c r="J12" t="s"/>
       <c r="K12" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="L12" t="n">
-        <v>16.72</v>
-      </c>
-      <c r="M12" t="s"/>
+        <v>0</v>
+      </c>
+      <c r="L12" t="s"/>
+      <c r="M12" t="n">
+        <v>16.24</v>
+      </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1" t="n"/>
@@ -830,26 +838,30 @@
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s"/>
-      <c r="E13" t="s"/>
+      <c r="D13" t="n">
+        <v>28.51</v>
+      </c>
+      <c r="E13" t="n">
+        <v>90.87</v>
+      </c>
       <c r="F13" t="n">
-        <v>13.24</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>98.64</v>
       </c>
       <c r="H13" t="s"/>
-      <c r="I13" t="s"/>
-      <c r="J13" t="n">
-        <v>48.64</v>
-      </c>
+      <c r="I13" t="n">
+        <v>13.71</v>
+      </c>
+      <c r="J13" t="s"/>
       <c r="K13" t="n">
         <v>0.01</v>
       </c>
-      <c r="L13" t="n">
-        <v>13.23</v>
-      </c>
-      <c r="M13" t="s"/>
+      <c r="L13" t="s"/>
+      <c r="M13" t="n">
+        <v>13.72</v>
+      </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1" t="n"/>
@@ -857,26 +869,30 @@
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s"/>
-      <c r="E14" t="s"/>
+      <c r="D14" t="n">
+        <v>90.87</v>
+      </c>
+      <c r="E14" t="n">
+        <v>43.75</v>
+      </c>
       <c r="F14" t="n">
-        <v>16.18</v>
+        <v>-150</v>
       </c>
       <c r="G14" t="n">
-        <v>-150</v>
+        <v>87.16</v>
       </c>
       <c r="H14" t="s"/>
-      <c r="I14" t="s"/>
-      <c r="J14" t="n">
-        <v>37.16</v>
-      </c>
+      <c r="I14" t="n">
+        <v>15.72</v>
+      </c>
+      <c r="J14" t="s"/>
       <c r="K14" t="n">
         <v>0</v>
       </c>
-      <c r="L14" t="n">
-        <v>16.18</v>
-      </c>
-      <c r="M14" t="s"/>
+      <c r="L14" t="s"/>
+      <c r="M14" t="n">
+        <v>15.72</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
@@ -888,24 +904,28 @@
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D15" t="s"/>
-      <c r="E15" t="s"/>
+      <c r="D15" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1.89</v>
+      </c>
       <c r="F15" t="n">
+        <v>-53.79</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s"/>
+      <c r="I15" t="n">
         <v>52.61</v>
       </c>
-      <c r="G15" t="n">
-        <v>-53.79</v>
-      </c>
-      <c r="H15" t="s"/>
-      <c r="I15" t="s"/>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
+      <c r="J15" t="s"/>
       <c r="K15" t="s"/>
-      <c r="L15" t="n">
+      <c r="L15" t="s"/>
+      <c r="M15" t="n">
         <v>52.61</v>
       </c>
-      <c r="M15" t="s"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1" t="n"/>
@@ -913,24 +933,28 @@
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="s"/>
-      <c r="E16" t="s"/>
+      <c r="D16" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="E16" t="n">
+        <v>15.46</v>
+      </c>
       <c r="F16" t="n">
+        <v>-53.31</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s"/>
+      <c r="I16" t="n">
         <v>66.88</v>
       </c>
-      <c r="G16" t="n">
-        <v>-53.31</v>
-      </c>
-      <c r="H16" t="s"/>
-      <c r="I16" t="s"/>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
+      <c r="J16" t="s"/>
       <c r="K16" t="s"/>
-      <c r="L16" t="n">
+      <c r="L16" t="s"/>
+      <c r="M16" t="n">
         <v>66.88</v>
       </c>
-      <c r="M16" t="s"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1" t="n"/>
@@ -938,24 +962,28 @@
       <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s"/>
-      <c r="E17" t="s"/>
+      <c r="D17" t="n">
+        <v>15.46</v>
+      </c>
+      <c r="E17" t="n">
+        <v>63.6</v>
+      </c>
       <c r="F17" t="n">
+        <v>-15.46</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="H17" t="s"/>
+      <c r="I17" t="n">
         <v>62.04</v>
       </c>
-      <c r="G17" t="n">
-        <v>-15.46</v>
-      </c>
-      <c r="H17" t="s"/>
-      <c r="I17" t="s"/>
-      <c r="J17" t="n">
-        <v>1.56</v>
-      </c>
+      <c r="J17" t="s"/>
       <c r="K17" t="s"/>
-      <c r="L17" t="n">
+      <c r="L17" t="s"/>
+      <c r="M17" t="n">
         <v>62.04</v>
       </c>
-      <c r="M17" t="s"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1" t="n"/>
@@ -963,24 +991,28 @@
       <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D18" t="s"/>
-      <c r="E18" t="s"/>
+      <c r="D18" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.89</v>
+      </c>
       <c r="F18" t="n">
+        <v>-469.67</v>
+      </c>
+      <c r="G18" t="n">
+        <v>351.04</v>
+      </c>
+      <c r="H18" t="s"/>
+      <c r="I18" t="n">
         <v>56.92</v>
       </c>
-      <c r="G18" t="n">
-        <v>-469.67</v>
-      </c>
-      <c r="H18" t="s"/>
-      <c r="I18" t="s"/>
-      <c r="J18" t="n">
-        <v>351.04</v>
-      </c>
+      <c r="J18" t="s"/>
       <c r="K18" t="s"/>
-      <c r="L18" t="n">
+      <c r="L18" t="s"/>
+      <c r="M18" t="n">
         <v>56.92</v>
       </c>
-      <c r="M18" t="s"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
@@ -992,32 +1024,32 @@
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" t="s"/>
+      <c r="D19" t="n">
+        <v>1.28</v>
+      </c>
       <c r="E19" t="n">
         <v>210.16</v>
       </c>
       <c r="F19" t="n">
-        <v>8.289999999999999</v>
+        <v>-150</v>
       </c>
       <c r="G19" t="n">
-        <v>-150</v>
+        <v>98.39</v>
       </c>
       <c r="H19" t="n">
-        <v>252.18</v>
+        <v>252.19</v>
       </c>
       <c r="I19" t="n">
-        <v>1.28</v>
-      </c>
-      <c r="J19" t="n">
-        <v>98.38</v>
-      </c>
+        <v>8.15</v>
+      </c>
+      <c r="J19" t="s"/>
       <c r="K19" t="n">
         <v>0.15</v>
       </c>
-      <c r="L19" t="n">
-        <v>8.140000000000001</v>
-      </c>
-      <c r="M19" t="s"/>
+      <c r="L19" t="s"/>
+      <c r="M19" t="n">
+        <v>8.300000000000001</v>
+      </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="n"/>
@@ -1025,32 +1057,32 @@
       <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D20" t="s"/>
+      <c r="D20" t="n">
+        <v>210.16</v>
+      </c>
       <c r="E20" t="n">
         <v>5.16</v>
       </c>
       <c r="F20" t="n">
-        <v>9.130000000000001</v>
+        <v>-430</v>
       </c>
       <c r="G20" t="n">
-        <v>-430</v>
+        <v>81.95999999999999</v>
       </c>
       <c r="H20" t="n">
         <v>133.91</v>
       </c>
       <c r="I20" t="n">
-        <v>210.16</v>
-      </c>
-      <c r="J20" t="n">
-        <v>81.94</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="J20" t="s"/>
       <c r="K20" t="n">
         <v>0.14</v>
       </c>
-      <c r="L20" t="n">
-        <v>8.99</v>
-      </c>
-      <c r="M20" t="s"/>
+      <c r="L20" t="s"/>
+      <c r="M20" t="n">
+        <v>9.140000000000001</v>
+      </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="n"/>
@@ -1058,32 +1090,32 @@
       <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s"/>
+      <c r="D21" t="n">
+        <v>5.16</v>
+      </c>
       <c r="E21" t="n">
         <v>3.4</v>
       </c>
       <c r="F21" t="n">
-        <v>10.19</v>
+        <v>-260</v>
       </c>
       <c r="G21" t="n">
-        <v>-260</v>
+        <v>99.34</v>
       </c>
       <c r="H21" t="n">
         <v>148.69</v>
       </c>
       <c r="I21" t="n">
-        <v>5.16</v>
-      </c>
-      <c r="J21" t="n">
-        <v>99.33</v>
-      </c>
+        <v>9.99</v>
+      </c>
+      <c r="J21" t="s"/>
       <c r="K21" t="n">
         <v>0.21</v>
       </c>
-      <c r="L21" t="n">
-        <v>9.98</v>
-      </c>
-      <c r="M21" t="s"/>
+      <c r="L21" t="s"/>
+      <c r="M21" t="n">
+        <v>10.2</v>
+      </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1" t="n"/>
@@ -1091,32 +1123,32 @@
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D22" t="s"/>
+      <c r="D22" t="n">
+        <v>3.4</v>
+      </c>
       <c r="E22" t="n">
         <v>0.04</v>
       </c>
       <c r="F22" t="n">
-        <v>9.390000000000001</v>
+        <v>-160</v>
       </c>
       <c r="G22" t="n">
-        <v>-160</v>
+        <v>78.88</v>
       </c>
       <c r="H22" t="n">
-        <v>68.36</v>
+        <v>68.37</v>
       </c>
       <c r="I22" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="J22" t="n">
-        <v>78.87</v>
-      </c>
+        <v>9.199999999999999</v>
+      </c>
+      <c r="J22" t="s"/>
       <c r="K22" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="L22" t="n">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="M22" t="s"/>
+        <v>0.2</v>
+      </c>
+      <c r="L22" t="s"/>
+      <c r="M22" t="n">
+        <v>9.4</v>
+      </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
@@ -1128,29 +1160,33 @@
       <c r="C23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D23" t="s"/>
-      <c r="E23" t="s"/>
+      <c r="D23" t="n">
+        <v>30.29</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10.5</v>
+      </c>
       <c r="F23" t="n">
-        <v>132.23</v>
+        <v>-2085.7</v>
       </c>
       <c r="G23" t="n">
-        <v>-2085.7</v>
+        <v>203.4</v>
       </c>
       <c r="H23" t="n">
         <v>1730.27</v>
       </c>
-      <c r="I23" t="s"/>
+      <c r="I23" t="n">
+        <v>109.12</v>
+      </c>
       <c r="J23" t="n">
-        <v>203.4</v>
+        <v>22.81</v>
       </c>
       <c r="K23" t="n">
         <v>0.3</v>
       </c>
-      <c r="L23" t="n">
-        <v>109.12</v>
-      </c>
+      <c r="L23" t="s"/>
       <c r="M23" t="n">
-        <v>22.81</v>
+        <v>132.23</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1159,29 +1195,33 @@
       <c r="C24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D24" t="s"/>
-      <c r="E24" t="s"/>
+      <c r="D24" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>91.11</v>
+      </c>
       <c r="F24" t="n">
-        <v>179.32</v>
+        <v>-3267.94</v>
       </c>
       <c r="G24" t="n">
-        <v>-3267.94</v>
+        <v>354.41</v>
       </c>
       <c r="H24" t="n">
         <v>2814.81</v>
       </c>
-      <c r="I24" t="s"/>
+      <c r="I24" t="n">
+        <v>159.23</v>
+      </c>
       <c r="J24" t="n">
-        <v>354.41</v>
+        <v>19.94</v>
       </c>
       <c r="K24" t="n">
         <v>0.15</v>
       </c>
-      <c r="L24" t="n">
-        <v>159.23</v>
-      </c>
+      <c r="L24" t="s"/>
       <c r="M24" t="n">
-        <v>19.94</v>
+        <v>179.32</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1190,29 +1230,33 @@
       <c r="C25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D25" t="s"/>
-      <c r="E25" t="s"/>
+      <c r="D25" t="n">
+        <v>91.11</v>
+      </c>
+      <c r="E25" t="n">
+        <v>90.79000000000001</v>
+      </c>
       <c r="F25" t="n">
-        <v>153.9</v>
+        <v>-3445.12</v>
       </c>
       <c r="G25" t="n">
-        <v>-3445.12</v>
+        <v>186.96</v>
       </c>
       <c r="H25" t="n">
         <v>3103.95</v>
       </c>
-      <c r="I25" t="s"/>
+      <c r="I25" t="n">
+        <v>128.56</v>
+      </c>
       <c r="J25" t="n">
-        <v>186.96</v>
+        <v>25.16</v>
       </c>
       <c r="K25" t="n">
         <v>0.18</v>
       </c>
-      <c r="L25" t="n">
-        <v>128.56</v>
-      </c>
+      <c r="L25" t="s"/>
       <c r="M25" t="n">
-        <v>25.16</v>
+        <v>153.9</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1221,29 +1265,33 @@
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D26" t="s"/>
-      <c r="E26" t="s"/>
+      <c r="D26" t="n">
+        <v>90.79000000000001</v>
+      </c>
+      <c r="E26" t="n">
+        <v>44.83</v>
+      </c>
       <c r="F26" t="n">
-        <v>132.35</v>
+        <v>-2851.35</v>
       </c>
       <c r="G26" t="n">
-        <v>-2796.92</v>
+        <v>283.05</v>
       </c>
       <c r="H26" t="n">
         <v>2369.27</v>
       </c>
-      <c r="I26" t="s"/>
+      <c r="I26" t="n">
+        <v>127.68</v>
+      </c>
       <c r="J26" t="n">
-        <v>258.94</v>
+        <v>25.26</v>
       </c>
       <c r="K26" t="n">
         <v>0.12</v>
       </c>
-      <c r="L26" t="n">
-        <v>106.96</v>
-      </c>
+      <c r="L26" t="s"/>
       <c r="M26" t="n">
-        <v>25.26</v>
+        <v>153.07</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1259,21 +1307,21 @@
       <c r="D27" t="s"/>
       <c r="E27" t="s"/>
       <c r="F27" t="n">
+        <v>-2565.39</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1931.82</v>
+      </c>
+      <c r="H27" t="s"/>
+      <c r="I27" t="n">
         <v>16.01</v>
       </c>
-      <c r="G27" t="n">
-        <v>-2565.39</v>
-      </c>
-      <c r="H27" t="s"/>
-      <c r="I27" t="s"/>
-      <c r="J27" t="n">
-        <v>1931.82</v>
-      </c>
+      <c r="J27" t="s"/>
       <c r="K27" t="s"/>
-      <c r="L27" t="n">
+      <c r="L27" t="s"/>
+      <c r="M27" t="n">
         <v>16.01</v>
       </c>
-      <c r="M27" t="s"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1" t="n"/>
@@ -1284,21 +1332,21 @@
       <c r="D28" t="s"/>
       <c r="E28" t="s"/>
       <c r="F28" t="n">
+        <v>-2383.37</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2382.13</v>
+      </c>
+      <c r="H28" t="s"/>
+      <c r="I28" t="n">
         <v>23.16</v>
       </c>
-      <c r="G28" t="n">
-        <v>-2383.37</v>
-      </c>
-      <c r="H28" t="s"/>
-      <c r="I28" t="s"/>
-      <c r="J28" t="n">
-        <v>2382.13</v>
-      </c>
+      <c r="J28" t="s"/>
       <c r="K28" t="s"/>
-      <c r="L28" t="n">
+      <c r="L28" t="s"/>
+      <c r="M28" t="n">
         <v>23.16</v>
       </c>
-      <c r="M28" t="s"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="1" t="n"/>
@@ -1309,21 +1357,21 @@
       <c r="D29" t="s"/>
       <c r="E29" t="s"/>
       <c r="F29" t="n">
+        <v>-2202.76</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2161.08</v>
+      </c>
+      <c r="H29" t="s"/>
+      <c r="I29" t="n">
         <v>19.76</v>
       </c>
-      <c r="G29" t="n">
-        <v>-2202.76</v>
-      </c>
-      <c r="H29" t="s"/>
-      <c r="I29" t="s"/>
-      <c r="J29" t="n">
-        <v>2161.08</v>
-      </c>
+      <c r="J29" t="s"/>
       <c r="K29" t="s"/>
-      <c r="L29" t="n">
+      <c r="L29" t="s"/>
+      <c r="M29" t="n">
         <v>19.76</v>
       </c>
-      <c r="M29" t="s"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="1" t="n"/>
@@ -1334,21 +1382,21 @@
       <c r="D30" t="s"/>
       <c r="E30" t="s"/>
       <c r="F30" t="n">
+        <v>-1972.52</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1953.53</v>
+      </c>
+      <c r="H30" t="s"/>
+      <c r="I30" t="n">
         <v>18.99</v>
       </c>
-      <c r="G30" t="n">
-        <v>-1972.52</v>
-      </c>
-      <c r="H30" t="s"/>
-      <c r="I30" t="s"/>
-      <c r="J30" t="n">
-        <v>1953.53</v>
-      </c>
+      <c r="J30" t="s"/>
       <c r="K30" t="s"/>
-      <c r="L30" t="n">
+      <c r="L30" t="s"/>
+      <c r="M30" t="n">
         <v>18.99</v>
       </c>
-      <c r="M30" t="s"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
@@ -1360,24 +1408,28 @@
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D31" t="s"/>
-      <c r="E31" t="s"/>
+      <c r="D31" t="n">
+        <v>1224.58</v>
+      </c>
+      <c r="E31" t="n">
+        <v>63.2</v>
+      </c>
       <c r="F31" t="n">
+        <v>3684.29</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2483.38</v>
+      </c>
+      <c r="H31" t="s"/>
+      <c r="I31" t="n">
         <v>39.53</v>
       </c>
-      <c r="G31" t="n">
-        <v>3684.29</v>
-      </c>
-      <c r="H31" t="s"/>
-      <c r="I31" t="s"/>
-      <c r="J31" t="n">
-        <v>2483.38</v>
-      </c>
+      <c r="J31" t="s"/>
       <c r="K31" t="s"/>
-      <c r="L31" t="n">
+      <c r="L31" t="s"/>
+      <c r="M31" t="n">
         <v>39.53</v>
       </c>
-      <c r="M31" t="s"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="1" t="n"/>
@@ -1385,24 +1437,28 @@
       <c r="C32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D32" t="s"/>
-      <c r="E32" t="s"/>
+      <c r="D32" t="n">
+        <v>-63.2</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
       <c r="F32" t="n">
+        <v>3181.35</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3082.15</v>
+      </c>
+      <c r="H32" t="s"/>
+      <c r="I32" t="n">
         <v>36</v>
       </c>
-      <c r="G32" t="n">
-        <v>3181.35</v>
-      </c>
-      <c r="H32" t="s"/>
-      <c r="I32" t="s"/>
-      <c r="J32" t="n">
-        <v>3082.15</v>
-      </c>
+      <c r="J32" t="s"/>
       <c r="K32" t="s"/>
-      <c r="L32" t="n">
+      <c r="L32" t="s"/>
+      <c r="M32" t="n">
         <v>36</v>
       </c>
-      <c r="M32" t="s"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="n"/>
@@ -1410,24 +1466,28 @@
       <c r="C33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D33" t="s"/>
-      <c r="E33" t="s"/>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
       <c r="F33" t="n">
+        <v>2267</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2239.91</v>
+      </c>
+      <c r="H33" t="s"/>
+      <c r="I33" t="n">
         <v>27.09</v>
       </c>
-      <c r="G33" t="n">
-        <v>2267</v>
-      </c>
-      <c r="H33" t="s"/>
-      <c r="I33" t="s"/>
-      <c r="J33" t="n">
-        <v>2239.91</v>
-      </c>
+      <c r="J33" t="s"/>
       <c r="K33" t="s"/>
-      <c r="L33" t="n">
+      <c r="L33" t="s"/>
+      <c r="M33" t="n">
         <v>27.09</v>
       </c>
-      <c r="M33" t="s"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1" t="n"/>
@@ -1435,24 +1495,28 @@
       <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D34" t="s"/>
-      <c r="E34" t="s"/>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.01</v>
+      </c>
       <c r="F34" t="n">
-        <v>29</v>
+        <v>2718.78</v>
       </c>
       <c r="G34" t="n">
-        <v>2670</v>
+        <v>2689.72</v>
       </c>
       <c r="H34" t="s"/>
-      <c r="I34" t="s"/>
-      <c r="J34" t="n">
-        <v>2641</v>
-      </c>
+      <c r="I34" t="n">
+        <v>29.06</v>
+      </c>
+      <c r="J34" t="s"/>
       <c r="K34" t="s"/>
-      <c r="L34" t="n">
-        <v>29</v>
-      </c>
-      <c r="M34" t="s"/>
+      <c r="L34" t="s"/>
+      <c r="M34" t="n">
+        <v>29.06</v>
+      </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
@@ -1467,24 +1531,24 @@
       <c r="D35" t="s"/>
       <c r="E35" t="s"/>
       <c r="F35" t="n">
-        <v>95.27</v>
+        <v>-4242.79</v>
       </c>
       <c r="G35" t="n">
-        <v>-4242.79</v>
+        <v>2024.53</v>
       </c>
       <c r="H35" t="n">
         <v>2131.78</v>
       </c>
-      <c r="I35" t="s"/>
+      <c r="I35" t="n">
+        <v>46.31</v>
+      </c>
       <c r="J35" t="n">
-        <v>2024.53</v>
+        <v>48.96</v>
       </c>
       <c r="K35" t="s"/>
-      <c r="L35" t="n">
-        <v>46.31</v>
-      </c>
+      <c r="L35" t="s"/>
       <c r="M35" t="n">
-        <v>48.96</v>
+        <v>95.27</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -1496,24 +1560,24 @@
       <c r="D36" t="s"/>
       <c r="E36" t="s"/>
       <c r="F36" t="n">
-        <v>81.75</v>
+        <v>-3510.8</v>
       </c>
       <c r="G36" t="n">
-        <v>-3510.8</v>
+        <v>2159.93</v>
       </c>
       <c r="H36" t="n">
         <v>1591.06</v>
       </c>
-      <c r="I36" t="s"/>
+      <c r="I36" t="n">
+        <v>47.95</v>
+      </c>
       <c r="J36" t="n">
-        <v>2159.93</v>
+        <v>33.8</v>
       </c>
       <c r="K36" t="s"/>
-      <c r="L36" t="n">
-        <v>47.95</v>
-      </c>
+      <c r="L36" t="s"/>
       <c r="M36" t="n">
-        <v>33.8</v>
+        <v>81.75</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -1525,24 +1589,24 @@
       <c r="D37" t="s"/>
       <c r="E37" t="s"/>
       <c r="F37" t="n">
-        <v>84.81999999999999</v>
+        <v>-4095.19</v>
       </c>
       <c r="G37" t="n">
-        <v>-4095.19</v>
+        <v>2486.32</v>
       </c>
       <c r="H37" t="n">
         <v>1434.85</v>
       </c>
-      <c r="I37" t="s"/>
+      <c r="I37" t="n">
+        <v>48.89</v>
+      </c>
       <c r="J37" t="n">
-        <v>2486.32</v>
+        <v>35.93</v>
       </c>
       <c r="K37" t="s"/>
-      <c r="L37" t="n">
-        <v>48.89</v>
-      </c>
+      <c r="L37" t="s"/>
       <c r="M37" t="n">
-        <v>35.93</v>
+        <v>84.81999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -1554,24 +1618,24 @@
       <c r="D38" t="s"/>
       <c r="E38" t="s"/>
       <c r="F38" t="n">
-        <v>67.62</v>
+        <v>-3432.68</v>
       </c>
       <c r="G38" t="n">
-        <v>-3432.68</v>
+        <v>1867.95</v>
       </c>
       <c r="H38" t="n">
         <v>1939.76</v>
       </c>
-      <c r="I38" t="s"/>
+      <c r="I38" t="n">
+        <v>35.62</v>
+      </c>
       <c r="J38" t="n">
-        <v>1867.95</v>
+        <v>32</v>
       </c>
       <c r="K38" t="s"/>
-      <c r="L38" t="n">
-        <v>35.62</v>
-      </c>
+      <c r="L38" t="s"/>
       <c r="M38" t="n">
-        <v>32</v>
+        <v>67.62</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -1587,24 +1651,24 @@
       <c r="D39" t="s"/>
       <c r="E39" t="s"/>
       <c r="F39" t="n">
-        <v>6.75</v>
+        <v>-170</v>
       </c>
       <c r="G39" t="n">
-        <v>-170</v>
+        <v>278.35</v>
       </c>
       <c r="H39" t="n">
         <v>168.63</v>
       </c>
-      <c r="I39" t="s"/>
+      <c r="I39" t="n">
+        <v>5.32</v>
+      </c>
       <c r="J39" t="n">
-        <v>278.35</v>
+        <v>1.42</v>
       </c>
       <c r="K39" t="s"/>
-      <c r="L39" t="n">
-        <v>5.32</v>
-      </c>
+      <c r="L39" t="s"/>
       <c r="M39" t="n">
-        <v>1.42</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -1616,24 +1680,24 @@
       <c r="D40" t="s"/>
       <c r="E40" t="s"/>
       <c r="F40" t="n">
-        <v>5.78</v>
+        <v>-562.89</v>
       </c>
       <c r="G40" t="n">
-        <v>-562.89</v>
+        <v>244.35</v>
       </c>
       <c r="H40" t="n">
         <v>186.28</v>
       </c>
-      <c r="I40" t="s"/>
+      <c r="I40" t="n">
+        <v>4.28</v>
+      </c>
       <c r="J40" t="n">
-        <v>244.35</v>
+        <v>1.5</v>
       </c>
       <c r="K40" t="s"/>
-      <c r="L40" t="n">
-        <v>4.28</v>
-      </c>
+      <c r="L40" t="s"/>
       <c r="M40" t="n">
-        <v>1.5</v>
+        <v>5.78</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -1645,24 +1709,24 @@
       <c r="D41" t="s"/>
       <c r="E41" t="s"/>
       <c r="F41" t="n">
-        <v>6</v>
+        <v>-455.26</v>
       </c>
       <c r="G41" t="n">
-        <v>-455.26</v>
+        <v>163.67</v>
       </c>
       <c r="H41" t="n">
         <v>263.32</v>
       </c>
-      <c r="I41" t="s"/>
+      <c r="I41" t="n">
+        <v>4.21</v>
+      </c>
       <c r="J41" t="n">
-        <v>163.67</v>
+        <v>1.79</v>
       </c>
       <c r="K41" t="s"/>
-      <c r="L41" t="n">
-        <v>4.21</v>
-      </c>
+      <c r="L41" t="s"/>
       <c r="M41" t="n">
-        <v>1.79</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -1674,24 +1738,24 @@
       <c r="D42" t="s"/>
       <c r="E42" t="s"/>
       <c r="F42" t="n">
-        <v>6.45</v>
+        <v>-455.74</v>
       </c>
       <c r="G42" t="n">
-        <v>-450.18</v>
+        <v>298.8</v>
       </c>
       <c r="H42" t="n">
         <v>153.38</v>
       </c>
-      <c r="I42" t="s"/>
+      <c r="I42" t="n">
+        <v>5.58</v>
+      </c>
       <c r="J42" t="n">
-        <v>298.8</v>
+        <v>1.04</v>
       </c>
       <c r="K42" t="s"/>
-      <c r="L42" t="n">
-        <v>5.41</v>
-      </c>
+      <c r="L42" t="s"/>
       <c r="M42" t="n">
-        <v>1.04</v>
+        <v>6.62</v>
       </c>
     </row>
   </sheetData>
@@ -1781,29 +1845,29 @@
         <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>-117.4</v>
+        <v>1.19</v>
       </c>
       <c r="D2" t="n">
         <v>0.77</v>
       </c>
       <c r="E2" t="n">
-        <v>576.46</v>
+        <v>-2670</v>
       </c>
       <c r="F2" t="n">
-        <v>-2670</v>
+        <v>975.71</v>
       </c>
       <c r="G2" t="s"/>
       <c r="H2" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="I2" t="n">
-        <v>975.71</v>
-      </c>
+        <v>693.86</v>
+      </c>
+      <c r="I2" t="s"/>
       <c r="J2" t="s"/>
       <c r="K2" t="n">
-        <v>693.86</v>
-      </c>
-      <c r="L2" t="s"/>
+        <v>-117.4</v>
+      </c>
+      <c r="L2" t="n">
+        <v>576.46</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
@@ -1815,21 +1879,21 @@
       <c r="C3" t="s"/>
       <c r="D3" t="s"/>
       <c r="E3" t="n">
+        <v>-8330</v>
+      </c>
+      <c r="F3" t="n">
+        <v>11410</v>
+      </c>
+      <c r="G3" t="s"/>
+      <c r="H3" t="n">
         <v>183.02</v>
       </c>
-      <c r="F3" t="n">
-        <v>-8330</v>
-      </c>
-      <c r="G3" t="s"/>
-      <c r="H3" t="s"/>
-      <c r="I3" t="n">
-        <v>11410</v>
-      </c>
+      <c r="I3" t="s"/>
       <c r="J3" t="s"/>
-      <c r="K3" t="n">
+      <c r="K3" t="s"/>
+      <c r="L3" t="n">
         <v>183.02</v>
       </c>
-      <c r="L3" t="s"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
@@ -1838,26 +1902,30 @@
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s"/>
-      <c r="D4" t="s"/>
+      <c r="C4" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="D4" t="n">
+        <v>43.75</v>
+      </c>
       <c r="E4" t="n">
-        <v>55.92</v>
+        <v>-400</v>
       </c>
       <c r="F4" t="n">
-        <v>-400</v>
+        <v>433.01</v>
       </c>
       <c r="G4" t="s"/>
-      <c r="H4" t="s"/>
-      <c r="I4" t="n">
-        <v>133.01</v>
-      </c>
+      <c r="H4" t="n">
+        <v>55.85</v>
+      </c>
+      <c r="I4" t="s"/>
       <c r="J4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="K4" t="n">
-        <v>55.89</v>
-      </c>
-      <c r="L4" t="s"/>
+        <v>0.02</v>
+      </c>
+      <c r="K4" t="s"/>
+      <c r="L4" t="n">
+        <v>55.87</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
@@ -1866,24 +1934,28 @@
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s"/>
-      <c r="D5" t="s"/>
+      <c r="C5" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.89</v>
+      </c>
       <c r="E5" t="n">
+        <v>-592.23</v>
+      </c>
+      <c r="F5" t="n">
+        <v>352.6</v>
+      </c>
+      <c r="G5" t="s"/>
+      <c r="H5" t="n">
         <v>238.45</v>
       </c>
-      <c r="F5" t="n">
-        <v>-592.23</v>
-      </c>
-      <c r="G5" t="s"/>
-      <c r="H5" t="s"/>
-      <c r="I5" t="n">
-        <v>352.6</v>
-      </c>
+      <c r="I5" t="s"/>
       <c r="J5" t="s"/>
-      <c r="K5" t="n">
+      <c r="K5" t="s"/>
+      <c r="L5" t="n">
         <v>238.45</v>
       </c>
-      <c r="L5" t="s"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
@@ -1892,32 +1964,32 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s"/>
+      <c r="C6" t="n">
+        <v>1.28</v>
+      </c>
       <c r="D6" t="n">
         <v>0.04</v>
       </c>
       <c r="E6" t="n">
-        <v>37</v>
+        <v>-1000</v>
       </c>
       <c r="F6" t="n">
-        <v>-1000</v>
+        <v>358.56</v>
       </c>
       <c r="G6" t="n">
-        <v>603.14</v>
+        <v>603.16</v>
       </c>
       <c r="H6" t="n">
-        <v>1.28</v>
-      </c>
-      <c r="I6" t="n">
-        <v>358.52</v>
-      </c>
+        <v>36.34</v>
+      </c>
+      <c r="I6" t="s"/>
       <c r="J6" t="n">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="K6" t="n">
-        <v>36.31</v>
-      </c>
-      <c r="L6" t="s"/>
+        <v>0.7</v>
+      </c>
+      <c r="K6" t="s"/>
+      <c r="L6" t="n">
+        <v>37.04</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
@@ -1926,29 +1998,33 @@
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s"/>
-      <c r="D7" t="s"/>
+      <c r="C7" t="n">
+        <v>30.29</v>
+      </c>
+      <c r="D7" t="n">
+        <v>44.83</v>
+      </c>
       <c r="E7" t="n">
-        <v>597.8099999999999</v>
+        <v>-11650.12</v>
       </c>
       <c r="F7" t="n">
-        <v>-11595.69</v>
+        <v>1027.83</v>
       </c>
       <c r="G7" t="n">
         <v>10018.3</v>
       </c>
-      <c r="H7" t="s"/>
+      <c r="H7" t="n">
+        <v>524.59</v>
+      </c>
       <c r="I7" t="n">
-        <v>1003.72</v>
+        <v>93.17</v>
       </c>
       <c r="J7" t="n">
         <v>0.76</v>
       </c>
-      <c r="K7" t="n">
-        <v>503.87</v>
-      </c>
+      <c r="K7" t="s"/>
       <c r="L7" t="n">
-        <v>93.17</v>
+        <v>618.53</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1961,21 +2037,21 @@
       <c r="C8" t="s"/>
       <c r="D8" t="s"/>
       <c r="E8" t="n">
+        <v>-9124.040000000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8428.559999999999</v>
+      </c>
+      <c r="G8" t="s"/>
+      <c r="H8" t="n">
         <v>77.92</v>
       </c>
-      <c r="F8" t="n">
-        <v>-9124.040000000001</v>
-      </c>
-      <c r="G8" t="s"/>
-      <c r="H8" t="s"/>
-      <c r="I8" t="n">
-        <v>8428.559999999999</v>
-      </c>
+      <c r="I8" t="s"/>
       <c r="J8" t="s"/>
-      <c r="K8" t="n">
+      <c r="K8" t="s"/>
+      <c r="L8" t="n">
         <v>77.92</v>
       </c>
-      <c r="L8" t="s"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
@@ -1984,24 +2060,28 @@
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s"/>
-      <c r="D9" t="s"/>
+      <c r="C9" t="n">
+        <v>1224.58</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.01</v>
+      </c>
       <c r="E9" t="n">
-        <v>131.62</v>
+        <v>11851.42</v>
       </c>
       <c r="F9" t="n">
-        <v>11802.64</v>
+        <v>10495.16</v>
       </c>
       <c r="G9" t="s"/>
-      <c r="H9" t="s"/>
-      <c r="I9" t="n">
-        <v>10446.44</v>
-      </c>
+      <c r="H9" t="n">
+        <v>131.68</v>
+      </c>
+      <c r="I9" t="s"/>
       <c r="J9" t="s"/>
-      <c r="K9" t="n">
-        <v>131.62</v>
-      </c>
-      <c r="L9" t="s"/>
+      <c r="K9" t="s"/>
+      <c r="L9" t="n">
+        <v>131.68</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
@@ -2013,24 +2093,24 @@
       <c r="C10" t="s"/>
       <c r="D10" t="s"/>
       <c r="E10" t="n">
-        <v>329.46</v>
+        <v>-15281.46</v>
       </c>
       <c r="F10" t="n">
-        <v>-15281.46</v>
+        <v>8538.73</v>
       </c>
       <c r="G10" t="n">
         <v>7097.45</v>
       </c>
-      <c r="H10" t="s"/>
+      <c r="H10" t="n">
+        <v>178.77</v>
+      </c>
       <c r="I10" t="n">
-        <v>8538.73</v>
+        <v>150.69</v>
       </c>
       <c r="J10" t="s"/>
-      <c r="K10" t="n">
-        <v>178.77</v>
-      </c>
+      <c r="K10" t="s"/>
       <c r="L10" t="n">
-        <v>150.69</v>
+        <v>329.46</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2043,24 +2123,24 @@
       <c r="C11" t="s"/>
       <c r="D11" t="s"/>
       <c r="E11" t="n">
-        <v>24.98</v>
+        <v>-1643.89</v>
       </c>
       <c r="F11" t="n">
-        <v>-1638.33</v>
+        <v>985.17</v>
       </c>
       <c r="G11" t="n">
         <v>771.62</v>
       </c>
-      <c r="H11" t="s"/>
+      <c r="H11" t="n">
+        <v>19.39</v>
+      </c>
       <c r="I11" t="n">
-        <v>985.17</v>
+        <v>5.76</v>
       </c>
       <c r="J11" t="s"/>
-      <c r="K11" t="n">
-        <v>19.22</v>
-      </c>
+      <c r="K11" t="s"/>
       <c r="L11" t="n">
-        <v>5.76</v>
+        <v>25.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>